<commit_message>
moved css and html pages into their own folder and updated paths, also began index page
</commit_message>
<xml_diff>
--- a/documentation/CISC480-Charter-GroupC.xlsx
+++ b/documentation/CISC480-Charter-GroupC.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10905"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uofstthomasmn-my.sharepoint.com/personal/heff5015_stthomas_edu/Documents/Fall_2025/CISC_480/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uofstthomasmn-my.sharepoint.com/personal/heff5015_stthomas_edu/Documents/Fall_2025/CISC-480-Project1/documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BF5421C9-B895-E248-A7B2-1729A9D28AA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="37" documentId="8_{BF5421C9-B895-E248-A7B2-1729A9D28AA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F0F86714-FB95-3941-BB8C-E83707B971D2}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -278,10 +278,10 @@
                   <c:v>45930</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>45950</c:v>
+                  <c:v>45948</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>45953</c:v>
+                  <c:v>45954</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -358,7 +358,7 @@
                   <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>4</c:v>
@@ -1112,10 +1112,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -1436,7 +1432,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1524,10 +1520,10 @@
         <v>7</v>
       </c>
       <c r="B5" s="2">
-        <v>45950</v>
+        <v>45948</v>
       </c>
       <c r="C5" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D5" s="2">
         <f>WORKDAY(B5,C5)</f>
@@ -1535,7 +1531,7 @@
       </c>
       <c r="E5" s="1">
         <f>D5-B5</f>
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -1543,14 +1539,14 @@
         <v>8</v>
       </c>
       <c r="B6" s="2">
-        <v>45953</v>
+        <v>45954</v>
       </c>
       <c r="C6" s="1">
         <v>2</v>
       </c>
       <c r="D6" s="2">
         <f>WORKDAY(B6,C6)</f>
-        <v>45957</v>
+        <v>45958</v>
       </c>
       <c r="E6" s="1">
         <f>D6-B6</f>

</xml_diff>